<commit_message>
Finished hardware, started software
</commit_message>
<xml_diff>
--- a/Hardware/Star_BOM.xlsx
+++ b/Hardware/Star_BOM.xlsx
@@ -14,12 +14,13 @@
   <sheets>
     <sheet name="Star" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="143">
   <si>
     <t>Reference</t>
   </si>
@@ -288,12 +289,6 @@
     <t>0603</t>
   </si>
   <si>
-    <t>3220-10-0100-00</t>
-  </si>
-  <si>
-    <t>1175-1627-ND</t>
-  </si>
-  <si>
     <t>0.05"</t>
   </si>
   <si>
@@ -430,6 +425,30 @@
   </si>
   <si>
     <t>R1 R10 R12 R13 R15 R16 R18 R19 R21 R22 R24 R25 R27 R29 R3 R31 R32 R37 R39 R41 R42 R44 R5 R7 R8</t>
+  </si>
+  <si>
+    <t>C0603C104M5RACTU</t>
+  </si>
+  <si>
+    <t>399-7845-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C220F1GACTU</t>
+  </si>
+  <si>
+    <t>399-11145-1-ND</t>
+  </si>
+  <si>
+    <t>732-5374-ND</t>
+  </si>
+  <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>609-4613-1-ND</t>
+  </si>
+  <si>
+    <t>2x Qty</t>
   </si>
 </sst>
 </file>
@@ -1284,22 +1303,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G34"/>
+  <dimension ref="B2:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="85.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1307,636 +1326,779 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1">
+        <f>C3*2</f>
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>1022</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D34" si="0">C4*2</f>
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="1">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="1">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
         <v>23</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="2">
+        <v>62201021121</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C18" s="1">
         <v>13</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C19" s="1">
         <v>25</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" s="1">
         <v>20</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="G20" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="G22" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
         <v>42</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
         <v>44</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>45</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>80</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="G33" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" t="s">
+        <v>124</v>
+      </c>
+      <c r="G34" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="H34" t="s">
         <v>119</v>
-      </c>
-      <c r="E34" t="s">
-        <v>126</v>
-      </c>
-      <c r="F34" t="s">
-        <v>120</v>
-      </c>
-      <c r="G34" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>